<commit_message>
Added push button and LED
</commit_message>
<xml_diff>
--- a/Cost Estimate.xlsx
+++ b/Cost Estimate.xlsx
@@ -176,6 +176,7 @@
   <fonts count="5">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -196,6 +197,7 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
@@ -243,7 +245,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -256,7 +258,7 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -273,14 +275,6 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -305,10 +299,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="M51" activeCellId="0" pane="topLeft" sqref="M51"/>
+      <selection activeCell="D22" activeCellId="0" pane="topLeft" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -320,7 +314,7 @@
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -355,7 +349,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -393,7 +387,7 @@
         <v>0.03792</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="3">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -431,7 +425,7 @@
         <v>0.052</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="4">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
@@ -469,7 +463,7 @@
         <v>0.05276</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="5">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
@@ -507,7 +501,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="6">
       <c r="A6" s="0" t="n">
         <v>6</v>
       </c>
@@ -545,7 +539,7 @@
         <v>0.04959</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="7">
       <c r="A7" s="0" t="n">
         <v>7</v>
       </c>
@@ -583,7 +577,7 @@
         <v>12.538</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="8">
       <c r="A8" s="0" t="n">
         <v>8</v>
       </c>
@@ -621,7 +615,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="9">
       <c r="A9" s="0" t="n">
         <v>9</v>
       </c>
@@ -659,7 +653,7 @@
         <v>0.063</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="10">
       <c r="A10" s="0" t="n">
         <v>10</v>
       </c>
@@ -697,7 +691,7 @@
         <v>0.28772</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="11">
       <c r="A11" s="0" t="n">
         <v>11</v>
       </c>
@@ -735,7 +729,7 @@
         <v>0.86276</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="12">
       <c r="A12" s="0" t="n">
         <v>12</v>
       </c>
@@ -770,7 +764,7 @@
         <v>1.88</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="13">
       <c r="A13" s="0" t="n">
         <v>13</v>
       </c>
@@ -805,7 +799,7 @@
         <v>5.04</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="14">
       <c r="C14" s="0" t="s">
         <v>33</v>
       </c>
@@ -837,7 +831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="15">
       <c r="C15" s="0" t="s">
         <v>33</v>
       </c>
@@ -872,7 +866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="16">
       <c r="A16" s="0" t="n">
         <v>14</v>
       </c>
@@ -880,7 +874,7 @@
         <v>38</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="18">
       <c r="E18" s="3" t="s">
         <v>39</v>
       </c>
@@ -888,14 +882,14 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="19">
       <c r="F19" s="3" t="s">
         <v>40</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="20">
       <c r="F20" s="4" t="n">
         <v>50</v>
       </c>
@@ -906,7 +900,7 @@
         <v>250</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="21">
       <c r="E21" s="1" t="s">
         <v>41</v>
       </c>
@@ -923,7 +917,7 @@
         <v>22.43375</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="22">
       <c r="E22" s="1" t="s">
         <v>42</v>
       </c>
@@ -939,8 +933,12 @@
         <f aca="false">H21*H20</f>
         <v>5608.4375</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="24">
+      <c r="M22" s="0" t="n">
+        <f aca="false">2981.2/40</f>
+        <v>74.53</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="24">
       <c r="E24" s="3" t="s">
         <v>39</v>
       </c>
@@ -951,7 +949,7 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="25">
       <c r="F25" s="3" t="s">
         <v>43</v>
       </c>
@@ -963,7 +961,7 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="26">
       <c r="C26" s="5" t="s">
         <v>45</v>
       </c>
@@ -992,7 +990,7 @@
         <v>250</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="27">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="27">
       <c r="C27" s="5" t="s">
         <v>47</v>
       </c>
@@ -1002,249 +1000,253 @@
       <c r="E27" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="F27" s="8" t="inlineStr">
+      <c r="F27" s="2" t="inlineStr">
         <f aca="false">$E27-F$21-$D$27*$E27</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G27" s="8" t="inlineStr">
+      <c r="G27" s="2" t="inlineStr">
         <f aca="false">$E27-G$21-$D$27*$E27</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H27" s="8" t="inlineStr">
+      <c r="H27" s="2" t="inlineStr">
         <f aca="false">$E27-H$21-$D$27*$E27</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I27" s="8" t="inlineStr">
+      <c r="I27" s="2" t="inlineStr">
         <f aca="false">I$26*F27</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J27" s="8" t="inlineStr">
+      <c r="J27" s="2" t="inlineStr">
         <f aca="false">J$26*G27</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K27" s="8" t="inlineStr">
+      <c r="K27" s="2" t="inlineStr">
         <f aca="false">K$26*H27</f>
         <is>
           <t/>
         </is>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="28">
       <c r="E28" s="7" t="n">
         <v>35</v>
       </c>
-      <c r="F28" s="8" t="inlineStr">
+      <c r="F28" s="2" t="inlineStr">
         <f aca="false">$E28-F$21-$D$27*$E28</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G28" s="8" t="inlineStr">
+      <c r="G28" s="2" t="inlineStr">
         <f aca="false">$E28-G$21-$D$27*$E28</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H28" s="8" t="inlineStr">
+      <c r="H28" s="2" t="inlineStr">
         <f aca="false">$E28-H$21-$D$27*$E28</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I28" s="8" t="inlineStr">
+      <c r="I28" s="2" t="inlineStr">
         <f aca="false">I$26*F28</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J28" s="8" t="inlineStr">
+      <c r="J28" s="2" t="inlineStr">
         <f aca="false">J$26*G28</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K28" s="8" t="inlineStr">
+      <c r="K28" s="2" t="inlineStr">
         <f aca="false">K$26*H28</f>
         <is>
           <t/>
         </is>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="29">
+      <c r="M28" s="0" t="n">
+        <f aca="false">818.8/2981.2</f>
+        <v>0.274654501543003</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="29">
       <c r="E29" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="F29" s="8" t="inlineStr">
+      <c r="F29" s="2" t="inlineStr">
         <f aca="false">$E29-F$21-$D$27*$E29</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G29" s="8" t="inlineStr">
+      <c r="G29" s="2" t="inlineStr">
         <f aca="false">$E29-G$21-$D$27*$E29</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H29" s="8" t="inlineStr">
+      <c r="H29" s="2" t="inlineStr">
         <f aca="false">$E29-H$21-$D$27*$E29</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I29" s="8" t="inlineStr">
+      <c r="I29" s="2" t="inlineStr">
         <f aca="false">I$26*F29</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J29" s="8" t="inlineStr">
+      <c r="J29" s="2" t="inlineStr">
         <f aca="false">J$26*G29</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K29" s="8" t="inlineStr">
+      <c r="K29" s="2" t="inlineStr">
         <f aca="false">K$26*H29</f>
         <is>
           <t/>
         </is>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="30">
       <c r="E30" s="7" t="n">
         <v>45</v>
       </c>
-      <c r="F30" s="8" t="inlineStr">
+      <c r="F30" s="2" t="inlineStr">
         <f aca="false">$E30-F$21-$D$27*$E30</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G30" s="8" t="inlineStr">
+      <c r="G30" s="2" t="inlineStr">
         <f aca="false">$E30-G$21-$D$27*$E30</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H30" s="8" t="inlineStr">
+      <c r="H30" s="2" t="inlineStr">
         <f aca="false">$E30-H$21-$D$27*$E30</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I30" s="8" t="inlineStr">
+      <c r="I30" s="2" t="inlineStr">
         <f aca="false">I$26*F30</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J30" s="8" t="inlineStr">
+      <c r="J30" s="2" t="inlineStr">
         <f aca="false">J$26*G30</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K30" s="8" t="inlineStr">
+      <c r="K30" s="2" t="inlineStr">
         <f aca="false">K$26*H30</f>
         <is>
           <t/>
         </is>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="31">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="31">
       <c r="E31" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="F31" s="8" t="inlineStr">
+      <c r="F31" s="2" t="inlineStr">
         <f aca="false">$E31-F$21-$D$27*$E31</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G31" s="8" t="inlineStr">
+      <c r="G31" s="2" t="inlineStr">
         <f aca="false">$E31-G$21-$D$27*$E31</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H31" s="8" t="inlineStr">
+      <c r="H31" s="2" t="inlineStr">
         <f aca="false">$E31-H$21-$D$27*$E31</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I31" s="8" t="inlineStr">
+      <c r="I31" s="2" t="inlineStr">
         <f aca="false">I$26*F31</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J31" s="8" t="inlineStr">
+      <c r="J31" s="2" t="inlineStr">
         <f aca="false">J$26*G31</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K31" s="8" t="inlineStr">
+      <c r="K31" s="2" t="inlineStr">
         <f aca="false">K$26*H31</f>
         <is>
           <t/>
         </is>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="32">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="32">
       <c r="E32" s="7" t="n">
         <v>55</v>
       </c>
-      <c r="F32" s="8" t="inlineStr">
+      <c r="F32" s="2" t="inlineStr">
         <f aca="false">$E32-F$21-$D$27*$E32</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G32" s="8" t="inlineStr">
+      <c r="G32" s="2" t="inlineStr">
         <f aca="false">$E32-G$21-$D$27*$E32</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H32" s="8" t="inlineStr">
+      <c r="H32" s="2" t="inlineStr">
         <f aca="false">$E32-H$21-$D$27*$E32</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I32" s="8" t="inlineStr">
+      <c r="I32" s="2" t="inlineStr">
         <f aca="false">I$26*F32</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J32" s="8" t="inlineStr">
+      <c r="J32" s="2" t="inlineStr">
         <f aca="false">J$26*G32</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K32" s="8" t="inlineStr">
+      <c r="K32" s="2" t="inlineStr">
         <f aca="false">K$26*H32</f>
         <is>
           <t/>
         </is>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="34">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="34">
       <c r="E34" s="3" t="s">
         <v>48</v>
       </c>
@@ -1252,25 +1254,25 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="35">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="35">
       <c r="F35" s="3" t="s">
         <v>40</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="36">
-      <c r="F36" s="9" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="36">
+      <c r="F36" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="G36" s="9" t="n">
+      <c r="G36" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="H36" s="9" t="n">
+      <c r="H36" s="4" t="n">
         <v>250</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="37">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="37">
       <c r="E37" s="1" t="s">
         <v>41</v>
       </c>
@@ -1284,7 +1286,7 @@
         <v>35.91575</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="38">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="38">
       <c r="E38" s="1" t="s">
         <v>42</v>
       </c>
@@ -1298,13 +1300,13 @@
         <v>5608.4375</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="39">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="39">
       <c r="E39" s="1"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="40">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="40">
       <c r="E40" s="3" t="s">
         <v>48</v>
       </c>
@@ -1315,7 +1317,7 @@
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="41">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="41">
       <c r="F41" s="3" t="s">
         <v>43</v>
       </c>
@@ -1327,269 +1329,269 @@
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="42">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="42">
       <c r="E42" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F42" s="9" t="n">
+      <c r="F42" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="G42" s="9" t="n">
+      <c r="G42" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="H42" s="9" t="n">
+      <c r="H42" s="4" t="n">
         <v>250</v>
       </c>
-      <c r="I42" s="9" t="n">
+      <c r="I42" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="J42" s="9" t="n">
+      <c r="J42" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="K42" s="9" t="n">
+      <c r="K42" s="4" t="n">
         <v>250</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="43">
-      <c r="E43" s="10" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="43">
+      <c r="E43" s="8" t="n">
         <v>30</v>
       </c>
-      <c r="F43" s="8" t="inlineStr">
+      <c r="F43" s="2" t="inlineStr">
         <f aca="false">$E43-F$37-$D$27*$E43</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G43" s="8" t="inlineStr">
+      <c r="G43" s="2" t="inlineStr">
         <f aca="false">$E43-G$37-$D$27*$E43</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H43" s="8" t="inlineStr">
+      <c r="H43" s="2" t="inlineStr">
         <f aca="false">$E43-H$37-$D$27*$E43</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I43" s="8" t="inlineStr">
+      <c r="I43" s="2" t="inlineStr">
         <f aca="false">I$26*F43</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J43" s="8" t="inlineStr">
+      <c r="J43" s="2" t="inlineStr">
         <f aca="false">J$26*G43</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K43" s="8" t="inlineStr">
+      <c r="K43" s="2" t="inlineStr">
         <f aca="false">K$26*H43</f>
         <is>
           <t/>
         </is>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="44">
-      <c r="E44" s="10" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="44">
+      <c r="E44" s="8" t="n">
         <v>35</v>
       </c>
-      <c r="F44" s="8" t="inlineStr">
+      <c r="F44" s="2" t="inlineStr">
         <f aca="false">$E44-F$37-$D$27*$E44</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G44" s="8" t="inlineStr">
+      <c r="G44" s="2" t="inlineStr">
         <f aca="false">$E44-G$37-$D$27*$E44</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H44" s="8" t="inlineStr">
+      <c r="H44" s="2" t="inlineStr">
         <f aca="false">$E44-H$37-$D$27*$E44</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I44" s="8" t="inlineStr">
+      <c r="I44" s="2" t="inlineStr">
         <f aca="false">I$26*F44</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J44" s="8" t="inlineStr">
+      <c r="J44" s="2" t="inlineStr">
         <f aca="false">J$26*G44</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K44" s="8" t="inlineStr">
+      <c r="K44" s="2" t="inlineStr">
         <f aca="false">K$26*H44</f>
         <is>
           <t/>
         </is>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="45">
-      <c r="E45" s="10" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="45">
+      <c r="E45" s="8" t="n">
         <v>40</v>
       </c>
-      <c r="F45" s="8" t="inlineStr">
+      <c r="F45" s="2" t="inlineStr">
         <f aca="false">$E45-F$37-$D$27*$E45</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G45" s="8" t="inlineStr">
+      <c r="G45" s="2" t="inlineStr">
         <f aca="false">$E45-G$37-$D$27*$E45</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H45" s="8" t="inlineStr">
+      <c r="H45" s="2" t="inlineStr">
         <f aca="false">$E45-H$37-$D$27*$E45</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I45" s="8" t="inlineStr">
+      <c r="I45" s="2" t="inlineStr">
         <f aca="false">I$26*F45</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J45" s="8" t="inlineStr">
+      <c r="J45" s="2" t="inlineStr">
         <f aca="false">J$26*G45</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K45" s="8" t="inlineStr">
+      <c r="K45" s="2" t="inlineStr">
         <f aca="false">K$26*H45</f>
         <is>
           <t/>
         </is>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="46">
-      <c r="E46" s="10" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="46">
+      <c r="E46" s="8" t="n">
         <v>45</v>
       </c>
-      <c r="F46" s="8" t="inlineStr">
+      <c r="F46" s="2" t="inlineStr">
         <f aca="false">$E46-F$37-$D$27*$E46</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G46" s="8" t="inlineStr">
+      <c r="G46" s="2" t="inlineStr">
         <f aca="false">$E46-G$37-$D$27*$E46</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H46" s="8" t="inlineStr">
+      <c r="H46" s="2" t="inlineStr">
         <f aca="false">$E46-H$37-$D$27*$E46</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I46" s="8" t="inlineStr">
+      <c r="I46" s="2" t="inlineStr">
         <f aca="false">I$26*F46</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J46" s="8" t="inlineStr">
+      <c r="J46" s="2" t="inlineStr">
         <f aca="false">J$26*G46</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K46" s="8" t="inlineStr">
+      <c r="K46" s="2" t="inlineStr">
         <f aca="false">K$26*H46</f>
         <is>
           <t/>
         </is>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="47">
-      <c r="E47" s="10" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="47">
+      <c r="E47" s="8" t="n">
         <v>50</v>
       </c>
-      <c r="F47" s="8" t="inlineStr">
+      <c r="F47" s="2" t="inlineStr">
         <f aca="false">$E47-F$37-$D$27*$E47</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G47" s="8" t="inlineStr">
+      <c r="G47" s="2" t="inlineStr">
         <f aca="false">$E47-G$37-$D$27*$E47</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H47" s="8" t="inlineStr">
+      <c r="H47" s="2" t="inlineStr">
         <f aca="false">$E47-H$37-$D$27*$E47</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I47" s="8" t="inlineStr">
+      <c r="I47" s="2" t="inlineStr">
         <f aca="false">I$26*F47</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J47" s="8" t="inlineStr">
+      <c r="J47" s="2" t="inlineStr">
         <f aca="false">J$26*G47</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K47" s="8" t="inlineStr">
+      <c r="K47" s="2" t="inlineStr">
         <f aca="false">K$26*H47</f>
         <is>
           <t/>
         </is>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="48">
-      <c r="E48" s="10" t="n">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="48">
+      <c r="E48" s="8" t="n">
         <v>55</v>
       </c>
-      <c r="F48" s="8" t="inlineStr">
+      <c r="F48" s="2" t="inlineStr">
         <f aca="false">$E48-F$37-$D$27*$E48</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G48" s="8" t="inlineStr">
+      <c r="G48" s="2" t="inlineStr">
         <f aca="false">$E48-G$37-$D$27*$E48</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H48" s="8" t="inlineStr">
+      <c r="H48" s="2" t="inlineStr">
         <f aca="false">$E48-H$37-$D$27*$E48</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I48" s="8" t="inlineStr">
+      <c r="I48" s="2" t="inlineStr">
         <f aca="false">I$26*F48</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J48" s="8" t="inlineStr">
+      <c r="J48" s="2" t="inlineStr">
         <f aca="false">J$26*G48</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K48" s="8" t="inlineStr">
+      <c r="K48" s="2" t="inlineStr">
         <f aca="false">K$26*H48</f>
         <is>
           <t/>

</xml_diff>

<commit_message>
Worked on library code.
</commit_message>
<xml_diff>
--- a/Cost Estimate.xlsx
+++ b/Cost Estimate.xlsx
@@ -203,12 +203,18 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -245,12 +251,16 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -302,7 +312,7 @@
   <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D22" activeCellId="0" pane="topLeft" sqref="D22"/>
+      <selection activeCell="B8" activeCellId="0" pane="topLeft" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -359,30 +369,30 @@
       <c r="C2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="3" t="n">
         <v>0.166</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="3" t="n">
         <f aca="false">F2*E1</f>
         <v>0.166</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="H2" s="3" t="n">
         <v>0.0821</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="I2" s="3" t="n">
         <f aca="false">H2*E1</f>
         <v>0.0821</v>
       </c>
-      <c r="J2" s="2" t="n">
+      <c r="J2" s="3" t="n">
         <v>0.03792</v>
       </c>
-      <c r="K2" s="2" t="n">
+      <c r="K2" s="3" t="n">
         <f aca="false">J2*E2</f>
         <v>0.03792</v>
       </c>
@@ -397,32 +407,34 @@
       <c r="C3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="n">
         <v>0.164</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="3" t="n">
         <f aca="false">F3*E2</f>
         <v>0.164</v>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="H3" s="3" t="n">
         <v>0.081</v>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="I3" s="3" t="n">
         <f aca="false">H3*E2</f>
         <v>0.081</v>
       </c>
-      <c r="J3" s="2" t="n">
+      <c r="J3" s="3" t="n">
         <v>0.013</v>
       </c>
-      <c r="K3" s="2" t="n">
+      <c r="K3" s="3" t="inlineStr">
         <f aca="false">J3*E3</f>
-        <v>0.052</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="4">
@@ -435,32 +447,38 @@
       <c r="C4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="F4" s="3" t="n">
         <v>0.0653</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="3" t="inlineStr">
         <f aca="false">F4*E3</f>
-        <v>0.2612</v>
-      </c>
-      <c r="H4" s="2" t="n">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H4" s="3" t="n">
         <v>0.04225</v>
       </c>
-      <c r="I4" s="2" t="n">
+      <c r="I4" s="3" t="inlineStr">
         <f aca="false">H4*E3</f>
-        <v>0.169</v>
-      </c>
-      <c r="J4" s="2" t="n">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J4" s="3" t="n">
         <v>0.05276</v>
       </c>
-      <c r="K4" s="2" t="n">
+      <c r="K4" s="3" t="inlineStr">
         <f aca="false">J4*E4</f>
-        <v>0.05276</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="5">
@@ -479,24 +497,28 @@
       <c r="E5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="3" t="n">
         <v>1.35</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="3" t="inlineStr">
         <f aca="false">F5*E4</f>
-        <v>1.35</v>
-      </c>
-      <c r="H5" s="2" t="n">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H5" s="3" t="n">
         <v>1.2</v>
       </c>
-      <c r="I5" s="2" t="n">
+      <c r="I5" s="3" t="inlineStr">
         <f aca="false">H5*E4</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="J5" s="3" t="n">
         <v>1.2</v>
       </c>
-      <c r="J5" s="2" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="K5" s="2" t="n">
+      <c r="K5" s="3" t="n">
         <f aca="false">J5*E5</f>
         <v>1.2</v>
       </c>
@@ -511,32 +533,34 @@
       <c r="C6" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F6" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" s="3" t="n">
         <v>0.0598</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="G6" s="3" t="n">
         <f aca="false">F6*E5</f>
         <v>0.0598</v>
       </c>
-      <c r="H6" s="2" t="n">
+      <c r="H6" s="3" t="n">
         <v>0.0331</v>
       </c>
-      <c r="I6" s="2" t="n">
+      <c r="I6" s="3" t="n">
         <f aca="false">H6*E5</f>
         <v>0.0331</v>
       </c>
-      <c r="J6" s="2" t="n">
+      <c r="J6" s="3" t="n">
         <v>0.01653</v>
       </c>
-      <c r="K6" s="2" t="n">
+      <c r="K6" s="3" t="inlineStr">
         <f aca="false">J6*E6</f>
-        <v>0.04959</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="7">
@@ -549,30 +573,30 @@
       <c r="C7" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="3" t="n">
         <v>12.65</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G7" s="3" t="n">
         <f aca="false">F7*E7</f>
         <v>12.65</v>
       </c>
-      <c r="H7" s="2" t="n">
+      <c r="H7" s="3" t="n">
         <v>12.55667</v>
       </c>
-      <c r="I7" s="2" t="n">
+      <c r="I7" s="3" t="n">
         <f aca="false">H7*E7</f>
         <v>12.55667</v>
       </c>
-      <c r="J7" s="2" t="n">
+      <c r="J7" s="3" t="n">
         <v>12.538</v>
       </c>
-      <c r="K7" s="2" t="n">
+      <c r="K7" s="3" t="n">
         <f aca="false">J7*E7</f>
         <v>12.538</v>
       </c>
@@ -593,24 +617,24 @@
       <c r="E8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="3" t="n">
         <v>1.48</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="3" t="n">
         <f aca="false">F8*E7</f>
         <v>1.48</v>
       </c>
-      <c r="H8" s="2" t="n">
+      <c r="H8" s="3" t="n">
         <v>0.37</v>
       </c>
-      <c r="I8" s="2" t="n">
+      <c r="I8" s="3" t="n">
         <f aca="false">H8*E7</f>
         <v>0.37</v>
       </c>
-      <c r="J8" s="2" t="n">
+      <c r="J8" s="3" t="n">
         <v>0.37</v>
       </c>
-      <c r="K8" s="2" t="n">
+      <c r="K8" s="3" t="n">
         <f aca="false">J8*E8</f>
         <v>0.37</v>
       </c>
@@ -625,30 +649,30 @@
       <c r="C9" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="3" t="n">
         <v>0.179</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="G9" s="3" t="n">
         <f aca="false">F9*E8</f>
         <v>0.179</v>
       </c>
-      <c r="H9" s="2" t="n">
+      <c r="H9" s="3" t="n">
         <v>0.105</v>
       </c>
-      <c r="I9" s="2" t="n">
+      <c r="I9" s="3" t="n">
         <f aca="false">H9*E8</f>
         <v>0.105</v>
       </c>
-      <c r="J9" s="2" t="n">
+      <c r="J9" s="3" t="n">
         <v>0.063</v>
       </c>
-      <c r="K9" s="2" t="n">
+      <c r="K9" s="3" t="n">
         <f aca="false">J9*E9</f>
         <v>0.063</v>
       </c>
@@ -663,30 +687,30 @@
       <c r="C10" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="3" t="n">
         <v>0.7652</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="G10" s="3" t="n">
         <f aca="false">F10*E9</f>
         <v>0.7652</v>
       </c>
-      <c r="H10" s="2" t="n">
+      <c r="H10" s="3" t="n">
         <v>0.3346</v>
       </c>
-      <c r="I10" s="2" t="n">
+      <c r="I10" s="3" t="n">
         <f aca="false">H10*E9</f>
         <v>0.3346</v>
       </c>
-      <c r="J10" s="2" t="n">
+      <c r="J10" s="3" t="n">
         <v>0.28772</v>
       </c>
-      <c r="K10" s="2" t="n">
+      <c r="K10" s="3" t="n">
         <f aca="false">J10*E10</f>
         <v>0.28772</v>
       </c>
@@ -701,30 +725,30 @@
       <c r="C11" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="3" t="n">
         <v>1.7656</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G11" s="3" t="n">
         <f aca="false">F11*E10</f>
         <v>1.7656</v>
       </c>
-      <c r="H11" s="2" t="n">
+      <c r="H11" s="3" t="n">
         <v>0.9205</v>
       </c>
-      <c r="I11" s="2" t="n">
+      <c r="I11" s="3" t="n">
         <f aca="false">H11*E10</f>
         <v>0.9205</v>
       </c>
-      <c r="J11" s="2" t="n">
+      <c r="J11" s="3" t="n">
         <v>0.86276</v>
       </c>
-      <c r="K11" s="2" t="n">
+      <c r="K11" s="3" t="n">
         <f aca="false">J11*E11</f>
         <v>0.86276</v>
       </c>
@@ -742,24 +766,24 @@
       <c r="E12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="3" t="n">
         <v>6.02</v>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="G12" s="3" t="n">
         <f aca="false">F12*E11</f>
         <v>6.02</v>
       </c>
-      <c r="H12" s="2" t="n">
+      <c r="H12" s="3" t="n">
         <v>3.46</v>
       </c>
-      <c r="I12" s="2" t="n">
+      <c r="I12" s="3" t="n">
         <f aca="false">H12*E11</f>
         <v>3.46</v>
       </c>
-      <c r="J12" s="2" t="n">
+      <c r="J12" s="3" t="n">
         <v>1.88</v>
       </c>
-      <c r="K12" s="2" t="n">
+      <c r="K12" s="3" t="n">
         <f aca="false">J12*E12</f>
         <v>1.88</v>
       </c>
@@ -777,24 +801,24 @@
       <c r="E13" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="F13" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="G13" s="2" t="n">
+      <c r="G13" s="3" t="n">
         <f aca="false">F13*E13</f>
         <v>21</v>
       </c>
-      <c r="H13" s="2" t="n">
+      <c r="H13" s="3" t="n">
         <v>10.5</v>
       </c>
-      <c r="I13" s="2" t="n">
+      <c r="I13" s="3" t="n">
         <f aca="false">H13*E13</f>
         <v>10.5</v>
       </c>
-      <c r="J13" s="2" t="n">
+      <c r="J13" s="3" t="n">
         <v>5.04</v>
       </c>
-      <c r="K13" s="2" t="n">
+      <c r="K13" s="3" t="n">
         <f aca="false">J13*E13</f>
         <v>5.04</v>
       </c>
@@ -809,24 +833,24 @@
       <c r="E14" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="3" t="n">
         <v>11.1</v>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="G14" s="3" t="n">
         <f aca="false">F14*E14</f>
         <v>0</v>
       </c>
-      <c r="H14" s="2" t="n">
+      <c r="H14" s="3" t="n">
         <v>5.82</v>
       </c>
-      <c r="I14" s="2" t="n">
+      <c r="I14" s="3" t="n">
         <f aca="false">H14*E14</f>
         <v>0</v>
       </c>
-      <c r="J14" s="2" t="n">
+      <c r="J14" s="3" t="n">
         <v>2.68</v>
       </c>
-      <c r="K14" s="2" t="n">
+      <c r="K14" s="3" t="n">
         <f aca="false">J14*E14</f>
         <v>0</v>
       </c>
@@ -841,27 +865,27 @@
       <c r="E15" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F15" s="3" t="n">
         <f aca="false">226.65/10</f>
         <v>22.665</v>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="G15" s="3" t="n">
         <f aca="false">F15*E15</f>
         <v>0</v>
       </c>
-      <c r="H15" s="2" t="n">
+      <c r="H15" s="3" t="n">
         <f aca="false">195.76/10</f>
         <v>19.576</v>
       </c>
-      <c r="I15" s="2" t="n">
+      <c r="I15" s="3" t="n">
         <f aca="false">H15*E15</f>
         <v>0</v>
       </c>
-      <c r="J15" s="2" t="n">
+      <c r="J15" s="3" t="n">
         <f aca="false">177.22/10</f>
         <v>17.722</v>
       </c>
-      <c r="K15" s="2" t="n">
+      <c r="K15" s="3" t="n">
         <f aca="false">J15*E15</f>
         <v>0</v>
       </c>
@@ -875,28 +899,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="18">
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="19">
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="20">
-      <c r="F20" s="4" t="n">
+      <c r="F20" s="5" t="n">
         <v>50</v>
       </c>
-      <c r="G20" s="4" t="n">
+      <c r="G20" s="5" t="n">
         <v>100</v>
       </c>
-      <c r="H20" s="4" t="n">
+      <c r="H20" s="5" t="n">
         <v>250</v>
       </c>
     </row>
@@ -904,34 +928,46 @@
       <c r="E21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="2" t="n">
+      <c r="F21" s="3" t="inlineStr">
         <f aca="false">SUM(G2:G16)</f>
-        <v>45.8608</v>
-      </c>
-      <c r="G21" s="2" t="n">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G21" s="3" t="inlineStr">
         <f aca="false">SUM(I2:I15)</f>
-        <v>29.81197</v>
-      </c>
-      <c r="H21" s="2" t="n">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H21" s="3" t="inlineStr">
         <f aca="false">SUM(K2:K15)</f>
-        <v>22.43375</v>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="22">
       <c r="E22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="2" t="n">
+      <c r="F22" s="3" t="inlineStr">
         <f aca="false">F20*F21</f>
-        <v>2293.04</v>
-      </c>
-      <c r="G22" s="2" t="n">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G22" s="3" t="inlineStr">
         <f aca="false">G20*G21</f>
-        <v>2981.197</v>
-      </c>
-      <c r="H22" s="2" t="n">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H22" s="3" t="inlineStr">
         <f aca="false">H21*H20</f>
-        <v>5608.4375</v>
+        <is>
+          <t/>
+        </is>
       </c>
       <c r="M22" s="0" t="n">
         <f aca="false">2981.2/40</f>
@@ -939,33 +975,33 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="24">
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="25">
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3" t="s">
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="26">
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="6" t="n">
+      <c r="D26" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E26" s="1" t="s">
@@ -991,46 +1027,46 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="27">
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D27" s="6" t="n">
+      <c r="D27" s="7" t="n">
         <v>0.05</v>
       </c>
-      <c r="E27" s="7" t="n">
+      <c r="E27" s="8" t="n">
         <v>30</v>
       </c>
-      <c r="F27" s="2" t="inlineStr">
+      <c r="F27" s="3" t="inlineStr">
         <f aca="false">$E27-F$21-$D$27*$E27</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G27" s="2" t="inlineStr">
+      <c r="G27" s="3" t="inlineStr">
         <f aca="false">$E27-G$21-$D$27*$E27</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H27" s="2" t="inlineStr">
+      <c r="H27" s="3" t="inlineStr">
         <f aca="false">$E27-H$21-$D$27*$E27</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I27" s="2" t="inlineStr">
+      <c r="I27" s="3" t="inlineStr">
         <f aca="false">I$26*F27</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J27" s="2" t="inlineStr">
+      <c r="J27" s="3" t="inlineStr">
         <f aca="false">J$26*G27</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K27" s="2" t="inlineStr">
+      <c r="K27" s="3" t="inlineStr">
         <f aca="false">K$26*H27</f>
         <is>
           <t/>
@@ -1038,40 +1074,40 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="28">
-      <c r="E28" s="7" t="n">
+      <c r="E28" s="8" t="n">
         <v>35</v>
       </c>
-      <c r="F28" s="2" t="inlineStr">
+      <c r="F28" s="3" t="inlineStr">
         <f aca="false">$E28-F$21-$D$27*$E28</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G28" s="2" t="inlineStr">
+      <c r="G28" s="3" t="inlineStr">
         <f aca="false">$E28-G$21-$D$27*$E28</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H28" s="2" t="inlineStr">
+      <c r="H28" s="3" t="inlineStr">
         <f aca="false">$E28-H$21-$D$27*$E28</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I28" s="2" t="inlineStr">
+      <c r="I28" s="3" t="inlineStr">
         <f aca="false">I$26*F28</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J28" s="2" t="inlineStr">
+      <c r="J28" s="3" t="inlineStr">
         <f aca="false">J$26*G28</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K28" s="2" t="inlineStr">
+      <c r="K28" s="3" t="inlineStr">
         <f aca="false">K$26*H28</f>
         <is>
           <t/>
@@ -1083,40 +1119,40 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="29">
-      <c r="E29" s="7" t="n">
+      <c r="E29" s="8" t="n">
         <v>40</v>
       </c>
-      <c r="F29" s="2" t="inlineStr">
+      <c r="F29" s="3" t="inlineStr">
         <f aca="false">$E29-F$21-$D$27*$E29</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G29" s="2" t="inlineStr">
+      <c r="G29" s="3" t="inlineStr">
         <f aca="false">$E29-G$21-$D$27*$E29</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H29" s="2" t="inlineStr">
+      <c r="H29" s="3" t="inlineStr">
         <f aca="false">$E29-H$21-$D$27*$E29</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I29" s="2" t="inlineStr">
+      <c r="I29" s="3" t="inlineStr">
         <f aca="false">I$26*F29</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J29" s="2" t="inlineStr">
+      <c r="J29" s="3" t="inlineStr">
         <f aca="false">J$26*G29</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K29" s="2" t="inlineStr">
+      <c r="K29" s="3" t="inlineStr">
         <f aca="false">K$26*H29</f>
         <is>
           <t/>
@@ -1124,40 +1160,40 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="30">
-      <c r="E30" s="7" t="n">
+      <c r="E30" s="8" t="n">
         <v>45</v>
       </c>
-      <c r="F30" s="2" t="inlineStr">
+      <c r="F30" s="3" t="inlineStr">
         <f aca="false">$E30-F$21-$D$27*$E30</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G30" s="2" t="inlineStr">
+      <c r="G30" s="3" t="inlineStr">
         <f aca="false">$E30-G$21-$D$27*$E30</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H30" s="2" t="inlineStr">
+      <c r="H30" s="3" t="inlineStr">
         <f aca="false">$E30-H$21-$D$27*$E30</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I30" s="2" t="inlineStr">
+      <c r="I30" s="3" t="inlineStr">
         <f aca="false">I$26*F30</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J30" s="2" t="inlineStr">
+      <c r="J30" s="3" t="inlineStr">
         <f aca="false">J$26*G30</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K30" s="2" t="inlineStr">
+      <c r="K30" s="3" t="inlineStr">
         <f aca="false">K$26*H30</f>
         <is>
           <t/>
@@ -1165,40 +1201,40 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="31">
-      <c r="E31" s="7" t="n">
+      <c r="E31" s="8" t="n">
         <v>50</v>
       </c>
-      <c r="F31" s="2" t="inlineStr">
+      <c r="F31" s="3" t="inlineStr">
         <f aca="false">$E31-F$21-$D$27*$E31</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G31" s="2" t="inlineStr">
+      <c r="G31" s="3" t="inlineStr">
         <f aca="false">$E31-G$21-$D$27*$E31</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H31" s="2" t="inlineStr">
+      <c r="H31" s="3" t="inlineStr">
         <f aca="false">$E31-H$21-$D$27*$E31</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I31" s="2" t="inlineStr">
+      <c r="I31" s="3" t="inlineStr">
         <f aca="false">I$26*F31</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J31" s="2" t="inlineStr">
+      <c r="J31" s="3" t="inlineStr">
         <f aca="false">J$26*G31</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K31" s="2" t="inlineStr">
+      <c r="K31" s="3" t="inlineStr">
         <f aca="false">K$26*H31</f>
         <is>
           <t/>
@@ -1206,40 +1242,40 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="32">
-      <c r="E32" s="7" t="n">
+      <c r="E32" s="8" t="n">
         <v>55</v>
       </c>
-      <c r="F32" s="2" t="inlineStr">
+      <c r="F32" s="3" t="inlineStr">
         <f aca="false">$E32-F$21-$D$27*$E32</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G32" s="2" t="inlineStr">
+      <c r="G32" s="3" t="inlineStr">
         <f aca="false">$E32-G$21-$D$27*$E32</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H32" s="2" t="inlineStr">
+      <c r="H32" s="3" t="inlineStr">
         <f aca="false">$E32-H$21-$D$27*$E32</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I32" s="2" t="inlineStr">
+      <c r="I32" s="3" t="inlineStr">
         <f aca="false">I$26*F32</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J32" s="2" t="inlineStr">
+      <c r="J32" s="3" t="inlineStr">
         <f aca="false">J$26*G32</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K32" s="2" t="inlineStr">
+      <c r="K32" s="3" t="inlineStr">
         <f aca="false">K$26*H32</f>
         <is>
           <t/>
@@ -1247,28 +1283,28 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="34">
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="35">
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="36">
-      <c r="F36" s="4" t="n">
+      <c r="F36" s="5" t="n">
         <v>50</v>
       </c>
-      <c r="G36" s="4" t="n">
+      <c r="G36" s="5" t="n">
         <v>100</v>
       </c>
-      <c r="H36" s="4" t="n">
+      <c r="H36" s="5" t="n">
         <v>250</v>
       </c>
     </row>
@@ -1276,13 +1312,13 @@
       <c r="E37" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F37" s="2" t="n">
+      <c r="F37" s="3" t="n">
         <v>58.6258</v>
       </c>
-      <c r="G37" s="2" t="n">
+      <c r="G37" s="3" t="n">
         <v>44.70797</v>
       </c>
-      <c r="H37" s="2" t="n">
+      <c r="H37" s="3" t="n">
         <v>35.91575</v>
       </c>
     </row>
@@ -1290,103 +1326,103 @@
       <c r="E38" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F38" s="2" t="n">
+      <c r="F38" s="3" t="n">
         <v>2293.04</v>
       </c>
-      <c r="G38" s="2" t="n">
+      <c r="G38" s="3" t="n">
         <v>2981.197</v>
       </c>
-      <c r="H38" s="2" t="n">
+      <c r="H38" s="3" t="n">
         <v>5608.4375</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="39">
       <c r="E39" s="1"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="40">
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="41">
-      <c r="F41" s="3" t="s">
+      <c r="F41" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3" t="s">
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="42">
       <c r="E42" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F42" s="4" t="n">
+      <c r="F42" s="5" t="n">
         <v>50</v>
       </c>
-      <c r="G42" s="4" t="n">
+      <c r="G42" s="5" t="n">
         <v>100</v>
       </c>
-      <c r="H42" s="4" t="n">
+      <c r="H42" s="5" t="n">
         <v>250</v>
       </c>
-      <c r="I42" s="4" t="n">
+      <c r="I42" s="5" t="n">
         <v>50</v>
       </c>
-      <c r="J42" s="4" t="n">
+      <c r="J42" s="5" t="n">
         <v>100</v>
       </c>
-      <c r="K42" s="4" t="n">
+      <c r="K42" s="5" t="n">
         <v>250</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="43">
-      <c r="E43" s="8" t="n">
+      <c r="E43" s="9" t="n">
         <v>30</v>
       </c>
-      <c r="F43" s="2" t="inlineStr">
+      <c r="F43" s="3" t="inlineStr">
         <f aca="false">$E43-F$37-$D$27*$E43</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G43" s="2" t="inlineStr">
+      <c r="G43" s="3" t="inlineStr">
         <f aca="false">$E43-G$37-$D$27*$E43</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H43" s="2" t="inlineStr">
+      <c r="H43" s="3" t="inlineStr">
         <f aca="false">$E43-H$37-$D$27*$E43</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I43" s="2" t="inlineStr">
+      <c r="I43" s="3" t="inlineStr">
         <f aca="false">I$26*F43</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J43" s="2" t="inlineStr">
+      <c r="J43" s="3" t="inlineStr">
         <f aca="false">J$26*G43</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K43" s="2" t="inlineStr">
+      <c r="K43" s="3" t="inlineStr">
         <f aca="false">K$26*H43</f>
         <is>
           <t/>
@@ -1394,40 +1430,40 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="44">
-      <c r="E44" s="8" t="n">
+      <c r="E44" s="9" t="n">
         <v>35</v>
       </c>
-      <c r="F44" s="2" t="inlineStr">
+      <c r="F44" s="3" t="inlineStr">
         <f aca="false">$E44-F$37-$D$27*$E44</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G44" s="2" t="inlineStr">
+      <c r="G44" s="3" t="inlineStr">
         <f aca="false">$E44-G$37-$D$27*$E44</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H44" s="2" t="inlineStr">
+      <c r="H44" s="3" t="inlineStr">
         <f aca="false">$E44-H$37-$D$27*$E44</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I44" s="2" t="inlineStr">
+      <c r="I44" s="3" t="inlineStr">
         <f aca="false">I$26*F44</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J44" s="2" t="inlineStr">
+      <c r="J44" s="3" t="inlineStr">
         <f aca="false">J$26*G44</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K44" s="2" t="inlineStr">
+      <c r="K44" s="3" t="inlineStr">
         <f aca="false">K$26*H44</f>
         <is>
           <t/>
@@ -1435,40 +1471,40 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="45">
-      <c r="E45" s="8" t="n">
+      <c r="E45" s="9" t="n">
         <v>40</v>
       </c>
-      <c r="F45" s="2" t="inlineStr">
+      <c r="F45" s="3" t="inlineStr">
         <f aca="false">$E45-F$37-$D$27*$E45</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G45" s="2" t="inlineStr">
+      <c r="G45" s="3" t="inlineStr">
         <f aca="false">$E45-G$37-$D$27*$E45</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H45" s="2" t="inlineStr">
+      <c r="H45" s="3" t="inlineStr">
         <f aca="false">$E45-H$37-$D$27*$E45</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I45" s="2" t="inlineStr">
+      <c r="I45" s="3" t="inlineStr">
         <f aca="false">I$26*F45</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J45" s="2" t="inlineStr">
+      <c r="J45" s="3" t="inlineStr">
         <f aca="false">J$26*G45</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K45" s="2" t="inlineStr">
+      <c r="K45" s="3" t="inlineStr">
         <f aca="false">K$26*H45</f>
         <is>
           <t/>
@@ -1476,40 +1512,40 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="46">
-      <c r="E46" s="8" t="n">
+      <c r="E46" s="9" t="n">
         <v>45</v>
       </c>
-      <c r="F46" s="2" t="inlineStr">
+      <c r="F46" s="3" t="inlineStr">
         <f aca="false">$E46-F$37-$D$27*$E46</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G46" s="2" t="inlineStr">
+      <c r="G46" s="3" t="inlineStr">
         <f aca="false">$E46-G$37-$D$27*$E46</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H46" s="2" t="inlineStr">
+      <c r="H46" s="3" t="inlineStr">
         <f aca="false">$E46-H$37-$D$27*$E46</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I46" s="2" t="inlineStr">
+      <c r="I46" s="3" t="inlineStr">
         <f aca="false">I$26*F46</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J46" s="2" t="inlineStr">
+      <c r="J46" s="3" t="inlineStr">
         <f aca="false">J$26*G46</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K46" s="2" t="inlineStr">
+      <c r="K46" s="3" t="inlineStr">
         <f aca="false">K$26*H46</f>
         <is>
           <t/>
@@ -1517,40 +1553,40 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="47">
-      <c r="E47" s="8" t="n">
+      <c r="E47" s="9" t="n">
         <v>50</v>
       </c>
-      <c r="F47" s="2" t="inlineStr">
+      <c r="F47" s="3" t="inlineStr">
         <f aca="false">$E47-F$37-$D$27*$E47</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G47" s="2" t="inlineStr">
+      <c r="G47" s="3" t="inlineStr">
         <f aca="false">$E47-G$37-$D$27*$E47</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H47" s="2" t="inlineStr">
+      <c r="H47" s="3" t="inlineStr">
         <f aca="false">$E47-H$37-$D$27*$E47</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I47" s="2" t="inlineStr">
+      <c r="I47" s="3" t="inlineStr">
         <f aca="false">I$26*F47</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J47" s="2" t="inlineStr">
+      <c r="J47" s="3" t="inlineStr">
         <f aca="false">J$26*G47</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K47" s="2" t="inlineStr">
+      <c r="K47" s="3" t="inlineStr">
         <f aca="false">K$26*H47</f>
         <is>
           <t/>
@@ -1558,40 +1594,40 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="48">
-      <c r="E48" s="8" t="n">
+      <c r="E48" s="9" t="n">
         <v>55</v>
       </c>
-      <c r="F48" s="2" t="inlineStr">
+      <c r="F48" s="3" t="inlineStr">
         <f aca="false">$E48-F$37-$D$27*$E48</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G48" s="2" t="inlineStr">
+      <c r="G48" s="3" t="inlineStr">
         <f aca="false">$E48-G$37-$D$27*$E48</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H48" s="2" t="inlineStr">
+      <c r="H48" s="3" t="inlineStr">
         <f aca="false">$E48-H$37-$D$27*$E48</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I48" s="2" t="inlineStr">
+      <c r="I48" s="3" t="inlineStr">
         <f aca="false">I$26*F48</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J48" s="2" t="inlineStr">
+      <c r="J48" s="3" t="inlineStr">
         <f aca="false">J$26*G48</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K48" s="2" t="inlineStr">
+      <c r="K48" s="3" t="inlineStr">
         <f aca="false">K$26*H48</f>
         <is>
           <t/>

</xml_diff>